<commit_message>
Grader IT excel file 70% submission file and score updated
</commit_message>
<xml_diff>
--- a/v2/Pegasus.Pages/TestData/Excel/ExcelFileFor70Percent/go_e01_grader_h3.xlsx
+++ b/v2/Pegasus.Pages/TestData/Excel/ExcelFileFor70Percent/go_e01_grader_h3.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7755"/>
@@ -9,9 +9,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="144525"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -63,12 +63,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,7 +263,17 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -298,6 +308,7 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -306,11 +317,13 @@
         <a:effectLst/>
       </c:spPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -381,6 +394,7 @@
               <a:bevelT w="25400" h="31750"/>
             </a:sp3d>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$4:$A$6</c:f>
@@ -487,6 +501,7 @@
               <a:bevelT w="25400" h="31750"/>
             </a:sp3d>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$4:$A$6</c:f>
@@ -593,6 +608,7 @@
               <a:bevelT w="25400" h="31750"/>
             </a:sp3d>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$4:$A$6</c:f>
@@ -703,6 +719,7 @@
               <a:bevelT w="25400" h="31750"/>
             </a:sp3d>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$4:$A$6</c:f>
@@ -739,19 +756,29 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="107187200"/>
-        <c:axId val="107975808"/>
+        <c:axId val="133240832"/>
+        <c:axId val="90427904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="107187200"/>
+        <c:axId val="133240832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -785,17 +812,19 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="107975808"/>
+        <c:crossAx val="90427904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107975808"/>
+        <c:axId val="90427904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -813,6 +842,7 @@
         </c:majorGridlines>
         <c:numFmt formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -840,7 +870,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="107187200"/>
+        <c:crossAx val="133240832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -855,6 +885,7 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -884,6 +915,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:gradFill flip="none" rotWithShape="1">
@@ -1774,27 +1806,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Retrospect" id="{5F128B03-DCCA-4EEB-AB3B-CF2899314A46}" vid="{3F1AAB62-24C6-49D2-8E01-B56FAC9A3DCD}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Retrospect" id="{5F128B03-DCCA-4EEB-AB3B-CF2899314A46}" vid="{3F1AAB62-24C6-49D2-8E01-B56FAC9A3DCD}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="8" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="23.25">
+    <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -1806,7 +1838,7 @@
       <c r="G1" s="18"/>
       <c r="H1" s="18"/>
     </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1">
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
@@ -1818,7 +1850,7 @@
       <c r="G2" s="19"/>
       <c r="H2" s="19"/>
     </row>
-    <row r="3" spans="1:8" ht="16.5" thickTop="1" thickBot="1">
+    <row r="3" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="17" t="s">
         <v>2</v>
       </c>
@@ -1841,7 +1873,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
@@ -1867,7 +1899,7 @@
       </c>
       <c r="H4" s="15"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1893,7 +1925,7 @@
       </c>
       <c r="H5" s="16"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -1918,7 +1950,7 @@
         <v>0.42551191502531821</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.75" thickBot="1">
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -1943,7 +1975,7 @@
         <v>2572974.39</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" thickTop="1"/>
+    <row r="8" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:H1"/>
@@ -1953,7 +1985,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
   <headerFooter>
-    <oddFooter>&amp;L&amp;F</oddFooter>
+    <oddFooter>&amp;A&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
   <extLst>
@@ -1978,10 +2010,6 @@
               <xm:sqref>H5</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
-              <xm:f>Sheet1!#REF!</xm:f>
-              <xm:sqref>#REF!</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
               <xm:f>Sheet1!B6:E6</xm:f>
               <xm:sqref>H6</xm:sqref>
             </x14:sparkline>

</xml_diff>